<commit_message>
Initial commit of new algorithm prototype
</commit_message>
<xml_diff>
--- a/Students table.xlsx
+++ b/Students table.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4c9fde938bfb13db/Рабочий стол/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malov\PycharmProjects\HueviyAlgosForProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Лист1!$A$1:$H$273</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1675,7 +1678,7 @@
   <dimension ref="A1:H273"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1713,7 +1716,7 @@
       <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="2">
         <v>0</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -8779,6 +8782,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H273"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>